<commit_message>
Updated method for formatting pairwise comparison outputs
</commit_message>
<xml_diff>
--- a/output/pearson_correlations.xlsx
+++ b/output/pearson_correlations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -50,10 +50,10 @@
     <t xml:space="preserve">1. STEM Career Interest</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00</t>
+    <t xml:space="preserve">6.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.94</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -62,13 +62,22 @@
     <t xml:space="preserve">2. General STEM Interest</t>
   </si>
   <si>
+    <t xml:space="preserve">6.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.73</t>
+  </si>
+  <si>
     <t xml:space="preserve">.70**</t>
   </si>
   <si>
     <t xml:space="preserve">3. STEM Belonging</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00</t>
+    <t xml:space="preserve">5.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.31</t>
   </si>
   <si>
     <t xml:space="preserve">.35**</t>
@@ -80,6 +89,12 @@
     <t xml:space="preserve">4. Identification with STEM</t>
   </si>
   <si>
+    <t xml:space="preserve">6.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.82</t>
+  </si>
+  <si>
     <t xml:space="preserve">.65**</t>
   </si>
   <si>
@@ -89,6 +104,12 @@
     <t xml:space="preserve">5. Threat</t>
   </si>
   <si>
+    <t xml:space="preserve">5.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.34</t>
+  </si>
+  <si>
     <t xml:space="preserve">-.04</t>
   </si>
   <si>
@@ -104,6 +125,12 @@
     <t xml:space="preserve">6. Challenge</t>
   </si>
   <si>
+    <t xml:space="preserve">5.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.15</t>
+  </si>
+  <si>
     <t xml:space="preserve">.47**</t>
   </si>
   <si>
@@ -122,6 +149,12 @@
     <t xml:space="preserve">7. STEM Self-Efficacy</t>
   </si>
   <si>
+    <t xml:space="preserve">5.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">.61**</t>
   </si>
   <si>
@@ -140,6 +173,12 @@
     <t xml:space="preserve">8. Person-Job Fit</t>
   </si>
   <si>
+    <t xml:space="preserve">5.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14</t>
+  </si>
+  <si>
     <t xml:space="preserve">.68**</t>
   </si>
   <si>
@@ -156,6 +195,12 @@
   </si>
   <si>
     <t xml:space="preserve">9. Confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.17</t>
   </si>
   <si>
     <t xml:space="preserve">.58**</t>
@@ -608,13 +653,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -640,19 +685,19 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
@@ -675,22 +720,22 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>14</v>
@@ -710,25 +755,25 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>14</v>
@@ -745,28 +790,28 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>14</v>
@@ -780,31 +825,31 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>14</v>
@@ -815,34 +860,34 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>14</v>
@@ -850,37 +895,37 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated correlation output format
</commit_message>
<xml_diff>
--- a/output/pearson_correlations.xlsx
+++ b/output/pearson_correlations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -32,21 +32,6 @@
     <t xml:space="preserve">X3</t>
   </si>
   <si>
-    <t xml:space="preserve">X4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X8</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. STEM Career Interest</t>
   </si>
   <si>
@@ -99,123 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve">.80**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Threat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.14*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.27**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Challenge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.47**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.56**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.46**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.51**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.43**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. STEM Self-Efficacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.61**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.43**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.53**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.37**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.59**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Person-Job Fit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.68**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.40**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.63**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.19**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.64**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9. Confidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.58**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.44**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.55**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-.32**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.71**</t>
   </si>
 </sst>
 </file>
@@ -597,335 +465,85 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>